<commit_message>
Added last tapioca of 2017
</commit_message>
<xml_diff>
--- a/posts/tapiocount_sheet.xlsx
+++ b/posts/tapiocount_sheet.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="tapiocount_sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="293">
   <si>
     <t>Purple Kow</t>
   </si>
@@ -897,6 +897,12 @@
   </si>
   <si>
     <t>dateLong</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4693/27703325939_75f0600371_z.jpg</t>
+  </si>
+  <si>
+    <t>The Yun Finest Green Tea</t>
   </si>
 </sst>
 </file>
@@ -904,8 +910,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="168" formatCode="mmmm\ d"/>
+    <numFmt numFmtId="165" formatCode="mmmm\ d"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -942,15 +948,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1230,12 +1234,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="10.83203125" style="4"/>
     <col min="3" max="3" width="20.1640625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
@@ -1248,7 +1253,7 @@
       <c r="A1" t="s">
         <v>282</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>283</v>
       </c>
       <c r="C1" t="s">
@@ -1278,7 +1283,7 @@
         <f>ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>42736</v>
       </c>
       <c r="C2" t="s">
@@ -1290,7 +1295,7 @@
       <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="2">
         <v>42736</v>
       </c>
     </row>
@@ -1299,7 +1304,7 @@
         <f t="shared" ref="A3:A66" si="0">ROW()-1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>42756</v>
       </c>
       <c r="C3" t="s">
@@ -1311,7 +1316,7 @@
       <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="2">
         <v>42756</v>
       </c>
     </row>
@@ -1320,7 +1325,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>42756</v>
       </c>
       <c r="C4" t="s">
@@ -1332,7 +1337,7 @@
       <c r="E4" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="2">
         <v>42756</v>
       </c>
     </row>
@@ -1341,7 +1346,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="4">
         <v>42762</v>
       </c>
       <c r="C5" t="s">
@@ -1353,7 +1358,7 @@
       <c r="E5" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="2">
         <v>42762</v>
       </c>
     </row>
@@ -1362,7 +1367,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="4">
         <v>42769</v>
       </c>
       <c r="C6" t="s">
@@ -1380,7 +1385,7 @@
       <c r="G6" t="s">
         <v>227</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="2">
         <v>42769</v>
       </c>
     </row>
@@ -1389,7 +1394,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="4">
         <v>42770</v>
       </c>
       <c r="C7" t="s">
@@ -1401,7 +1406,7 @@
       <c r="E7" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="2">
         <v>42770</v>
       </c>
     </row>
@@ -1410,7 +1415,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="4">
         <v>42770</v>
       </c>
       <c r="C8" t="s">
@@ -1422,7 +1427,7 @@
       <c r="E8" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="2">
         <v>42770</v>
       </c>
     </row>
@@ -1431,7 +1436,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="4">
         <v>42774</v>
       </c>
       <c r="C9" t="s">
@@ -1443,7 +1448,7 @@
       <c r="E9" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="2">
         <v>42774</v>
       </c>
     </row>
@@ -1452,7 +1457,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="4">
         <v>42779</v>
       </c>
       <c r="C10" t="s">
@@ -1467,7 +1472,7 @@
       <c r="F10" t="s">
         <v>226</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="2">
         <v>42779</v>
       </c>
     </row>
@@ -1476,24 +1481,24 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="5">
         <v>42784</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="7">
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="3">
         <v>42784</v>
       </c>
     </row>
@@ -1502,7 +1507,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="4">
         <v>42791</v>
       </c>
       <c r="C12" t="s">
@@ -1517,7 +1522,7 @@
       <c r="F12" t="s">
         <v>151</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="2">
         <v>42791</v>
       </c>
     </row>
@@ -1526,7 +1531,7 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="4">
         <v>42798</v>
       </c>
       <c r="C13" t="s">
@@ -1544,7 +1549,7 @@
       <c r="G13" t="s">
         <v>221</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="2">
         <v>42798</v>
       </c>
     </row>
@@ -1553,7 +1558,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="4">
         <v>42804</v>
       </c>
       <c r="C14" t="s">
@@ -1568,7 +1573,7 @@
       <c r="F14" t="s">
         <v>219</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="2">
         <v>42804</v>
       </c>
     </row>
@@ -1577,7 +1582,7 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="4">
         <v>42805</v>
       </c>
       <c r="C15" t="s">
@@ -1592,7 +1597,7 @@
       <c r="F15" t="s">
         <v>218</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="2">
         <v>42805</v>
       </c>
     </row>
@@ -1601,7 +1606,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="4">
         <v>42806</v>
       </c>
       <c r="C16" t="s">
@@ -1616,7 +1621,7 @@
       <c r="F16" t="s">
         <v>217</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="2">
         <v>42806</v>
       </c>
     </row>
@@ -1625,7 +1630,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="4">
         <v>42812</v>
       </c>
       <c r="C17" t="s">
@@ -1640,7 +1645,7 @@
       <c r="F17" t="s">
         <v>216</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="2">
         <v>42812</v>
       </c>
     </row>
@@ -1649,7 +1654,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="4">
         <v>42813</v>
       </c>
       <c r="C18" t="s">
@@ -1667,7 +1672,7 @@
       <c r="G18" t="s">
         <v>215</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="2">
         <v>42813</v>
       </c>
     </row>
@@ -1676,7 +1681,7 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="4">
         <v>42817</v>
       </c>
       <c r="C19" t="s">
@@ -1694,7 +1699,7 @@
       <c r="G19" t="s">
         <v>230</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="2">
         <v>42817</v>
       </c>
     </row>
@@ -1703,7 +1708,7 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="4">
         <v>42829</v>
       </c>
       <c r="C20" t="s">
@@ -1718,7 +1723,7 @@
       <c r="F20" t="s">
         <v>213</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="2">
         <v>42829</v>
       </c>
     </row>
@@ -1727,7 +1732,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="4">
         <v>42832</v>
       </c>
       <c r="C21" t="s">
@@ -1739,7 +1744,7 @@
       <c r="E21" t="s">
         <v>39</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="2">
         <v>42832</v>
       </c>
     </row>
@@ -1748,7 +1753,7 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="4">
         <v>42834</v>
       </c>
       <c r="C22" t="s">
@@ -1766,7 +1771,7 @@
       <c r="G22" t="s">
         <v>153</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="2">
         <v>42834</v>
       </c>
     </row>
@@ -1775,7 +1780,7 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="4">
         <v>42835</v>
       </c>
       <c r="C23" t="s">
@@ -1793,7 +1798,7 @@
       <c r="G23" t="s">
         <v>274</v>
       </c>
-      <c r="I23" s="6">
+      <c r="I23" s="2">
         <v>42835</v>
       </c>
     </row>
@@ -1802,7 +1807,7 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="4">
         <v>42836</v>
       </c>
       <c r="C24" t="s">
@@ -1817,7 +1822,7 @@
       <c r="F24" t="s">
         <v>235</v>
       </c>
-      <c r="I24" s="6">
+      <c r="I24" s="2">
         <v>42836</v>
       </c>
     </row>
@@ -1826,7 +1831,7 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="4">
         <v>42846</v>
       </c>
       <c r="C25" t="s">
@@ -1841,7 +1846,7 @@
       <c r="F25" t="s">
         <v>209</v>
       </c>
-      <c r="I25" s="6">
+      <c r="I25" s="2">
         <v>42846</v>
       </c>
     </row>
@@ -1850,7 +1855,7 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="4">
         <v>42848</v>
       </c>
       <c r="C26" t="s">
@@ -1865,7 +1870,7 @@
       <c r="F26" t="s">
         <v>208</v>
       </c>
-      <c r="I26" s="6">
+      <c r="I26" s="2">
         <v>42848</v>
       </c>
     </row>
@@ -1874,7 +1879,7 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="4">
         <v>42854</v>
       </c>
       <c r="C27" t="s">
@@ -1892,7 +1897,7 @@
       <c r="G27" t="s">
         <v>207</v>
       </c>
-      <c r="I27" s="6">
+      <c r="I27" s="2">
         <v>42854</v>
       </c>
     </row>
@@ -1901,7 +1906,7 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="4">
         <v>42855</v>
       </c>
       <c r="C28" t="s">
@@ -1916,7 +1921,7 @@
       <c r="F28" t="s">
         <v>233</v>
       </c>
-      <c r="I28" s="6">
+      <c r="I28" s="2">
         <v>42855</v>
       </c>
     </row>
@@ -1925,7 +1930,7 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="4">
         <v>42870</v>
       </c>
       <c r="C29" t="s">
@@ -1943,7 +1948,7 @@
       <c r="G29" t="s">
         <v>234</v>
       </c>
-      <c r="I29" s="6">
+      <c r="I29" s="2">
         <v>42870</v>
       </c>
     </row>
@@ -1952,7 +1957,7 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="4">
         <v>42877</v>
       </c>
       <c r="C30" t="s">
@@ -1967,7 +1972,7 @@
       <c r="F30" t="s">
         <v>206</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I30" s="2">
         <v>42877</v>
       </c>
     </row>
@@ -1976,7 +1981,7 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="4">
         <v>42880</v>
       </c>
       <c r="C31" t="s">
@@ -1991,7 +1996,7 @@
       <c r="F31" t="s">
         <v>238</v>
       </c>
-      <c r="I31" s="6">
+      <c r="I31" s="2">
         <v>42880</v>
       </c>
     </row>
@@ -2000,7 +2005,7 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="4">
         <v>42881</v>
       </c>
       <c r="C32" t="s">
@@ -2015,7 +2020,7 @@
       <c r="F32" t="s">
         <v>237</v>
       </c>
-      <c r="I32" s="6">
+      <c r="I32" s="2">
         <v>42881</v>
       </c>
     </row>
@@ -2024,7 +2029,7 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="4">
         <v>42890</v>
       </c>
       <c r="C33" t="s">
@@ -2039,7 +2044,7 @@
       <c r="F33" t="s">
         <v>236</v>
       </c>
-      <c r="I33" s="6">
+      <c r="I33" s="2">
         <v>42890</v>
       </c>
     </row>
@@ -2048,7 +2053,7 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="4">
         <v>42891</v>
       </c>
       <c r="C34" t="s">
@@ -2063,7 +2068,7 @@
       <c r="F34" t="s">
         <v>204</v>
       </c>
-      <c r="I34" s="6">
+      <c r="I34" s="2">
         <v>42891</v>
       </c>
     </row>
@@ -2072,7 +2077,7 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="4">
         <v>42891</v>
       </c>
       <c r="C35" t="s">
@@ -2087,7 +2092,7 @@
       <c r="F35" t="s">
         <v>203</v>
       </c>
-      <c r="I35" s="6">
+      <c r="I35" s="2">
         <v>42891</v>
       </c>
     </row>
@@ -2096,7 +2101,7 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="4">
         <v>42897</v>
       </c>
       <c r="C36" t="s">
@@ -2111,7 +2116,7 @@
       <c r="F36" t="s">
         <v>202</v>
       </c>
-      <c r="I36" s="6">
+      <c r="I36" s="2">
         <v>42897</v>
       </c>
     </row>
@@ -2120,7 +2125,7 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="4">
         <v>42899</v>
       </c>
       <c r="C37" t="s">
@@ -2135,7 +2140,7 @@
       <c r="F37" t="s">
         <v>201</v>
       </c>
-      <c r="I37" s="6">
+      <c r="I37" s="2">
         <v>42899</v>
       </c>
     </row>
@@ -2144,7 +2149,7 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="4">
         <v>42901</v>
       </c>
       <c r="C38" t="s">
@@ -2162,7 +2167,7 @@
       <c r="G38" t="s">
         <v>200</v>
       </c>
-      <c r="I38" s="6">
+      <c r="I38" s="2">
         <v>42901</v>
       </c>
     </row>
@@ -2171,7 +2176,7 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="4">
         <v>42902</v>
       </c>
       <c r="C39" t="s">
@@ -2186,7 +2191,7 @@
       <c r="F39" t="s">
         <v>198</v>
       </c>
-      <c r="I39" s="6">
+      <c r="I39" s="2">
         <v>42902</v>
       </c>
     </row>
@@ -2195,7 +2200,7 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="4">
         <v>42904</v>
       </c>
       <c r="C40" t="s">
@@ -2210,7 +2215,7 @@
       <c r="F40" t="s">
         <v>155</v>
       </c>
-      <c r="I40" s="6">
+      <c r="I40" s="2">
         <v>42904</v>
       </c>
     </row>
@@ -2219,7 +2224,7 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="4">
         <v>42914</v>
       </c>
       <c r="C41" t="s">
@@ -2234,7 +2239,7 @@
       <c r="F41" t="s">
         <v>197</v>
       </c>
-      <c r="I41" s="6">
+      <c r="I41" s="2">
         <v>42914</v>
       </c>
     </row>
@@ -2243,7 +2248,7 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="4">
         <v>42918</v>
       </c>
       <c r="C42" t="s">
@@ -2261,7 +2266,7 @@
       <c r="G42" t="s">
         <v>195</v>
       </c>
-      <c r="I42" s="6">
+      <c r="I42" s="2">
         <v>42918</v>
       </c>
     </row>
@@ -2270,7 +2275,7 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="4">
         <v>42919</v>
       </c>
       <c r="C43" t="s">
@@ -2285,7 +2290,7 @@
       <c r="F43" t="s">
         <v>194</v>
       </c>
-      <c r="I43" s="6">
+      <c r="I43" s="2">
         <v>42919</v>
       </c>
     </row>
@@ -2294,7 +2299,7 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="4">
         <v>42920</v>
       </c>
       <c r="C44" t="s">
@@ -2312,7 +2317,7 @@
       <c r="G44" t="s">
         <v>193</v>
       </c>
-      <c r="I44" s="6">
+      <c r="I44" s="2">
         <v>42920</v>
       </c>
     </row>
@@ -2321,7 +2326,7 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="4">
         <v>42924</v>
       </c>
       <c r="C45" t="s">
@@ -2333,7 +2338,7 @@
       <c r="E45" t="s">
         <v>42</v>
       </c>
-      <c r="I45" s="6">
+      <c r="I45" s="2">
         <v>42924</v>
       </c>
     </row>
@@ -2342,7 +2347,7 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="4">
         <v>42926</v>
       </c>
       <c r="C46" t="s">
@@ -2360,7 +2365,7 @@
       <c r="G46" t="s">
         <v>191</v>
       </c>
-      <c r="I46" s="6">
+      <c r="I46" s="2">
         <v>42926</v>
       </c>
     </row>
@@ -2369,7 +2374,7 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="4">
         <v>42927</v>
       </c>
       <c r="C47" t="s">
@@ -2384,7 +2389,7 @@
       <c r="F47" t="s">
         <v>189</v>
       </c>
-      <c r="I47" s="6">
+      <c r="I47" s="2">
         <v>42927</v>
       </c>
     </row>
@@ -2393,7 +2398,7 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="4">
         <v>42929</v>
       </c>
       <c r="C48" t="s">
@@ -2411,7 +2416,7 @@
       <c r="G48" t="s">
         <v>156</v>
       </c>
-      <c r="I48" s="6">
+      <c r="I48" s="2">
         <v>42929</v>
       </c>
     </row>
@@ -2420,7 +2425,7 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="4">
         <v>42930</v>
       </c>
       <c r="C49" t="s">
@@ -2438,7 +2443,7 @@
       <c r="G49" t="s">
         <v>157</v>
       </c>
-      <c r="I49" s="6">
+      <c r="I49" s="2">
         <v>42930</v>
       </c>
     </row>
@@ -2447,7 +2452,7 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="4">
         <v>42932</v>
       </c>
       <c r="C50" t="s">
@@ -2465,7 +2470,7 @@
       <c r="G50" t="s">
         <v>159</v>
       </c>
-      <c r="I50" s="6">
+      <c r="I50" s="2">
         <v>42932</v>
       </c>
     </row>
@@ -2474,7 +2479,7 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="4">
         <v>42934</v>
       </c>
       <c r="C51" t="s">
@@ -2489,7 +2494,7 @@
       <c r="F51" t="s">
         <v>182</v>
       </c>
-      <c r="I51" s="6">
+      <c r="I51" s="2">
         <v>42934</v>
       </c>
     </row>
@@ -2498,7 +2503,7 @@
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="4">
         <v>42936</v>
       </c>
       <c r="C52" t="s">
@@ -2513,7 +2518,7 @@
       <c r="F52" t="s">
         <v>160</v>
       </c>
-      <c r="I52" s="6">
+      <c r="I52" s="2">
         <v>42936</v>
       </c>
     </row>
@@ -2522,7 +2527,7 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53" s="4">
         <v>42940</v>
       </c>
       <c r="C53" t="s">
@@ -2540,7 +2545,7 @@
       <c r="G53" t="s">
         <v>161</v>
       </c>
-      <c r="I53" s="6">
+      <c r="I53" s="2">
         <v>42940</v>
       </c>
     </row>
@@ -2549,7 +2554,7 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54" s="4">
         <v>42945</v>
       </c>
       <c r="C54" t="s">
@@ -2564,7 +2569,7 @@
       <c r="F54" t="s">
         <v>178</v>
       </c>
-      <c r="I54" s="6">
+      <c r="I54" s="2">
         <v>42945</v>
       </c>
     </row>
@@ -2573,7 +2578,7 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="4">
         <v>42951</v>
       </c>
       <c r="C55" t="s">
@@ -2588,7 +2593,7 @@
       <c r="F55" t="s">
         <v>205</v>
       </c>
-      <c r="I55" s="6">
+      <c r="I55" s="2">
         <v>42951</v>
       </c>
     </row>
@@ -2597,7 +2602,7 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="4">
         <v>42951</v>
       </c>
       <c r="C56" t="s">
@@ -2612,7 +2617,7 @@
       <c r="F56" t="s">
         <v>176</v>
       </c>
-      <c r="I56" s="6">
+      <c r="I56" s="2">
         <v>42951</v>
       </c>
     </row>
@@ -2621,7 +2626,7 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="4">
         <v>42953</v>
       </c>
       <c r="C57" t="s">
@@ -2636,7 +2641,7 @@
       <c r="F57" t="s">
         <v>179</v>
       </c>
-      <c r="I57" s="6">
+      <c r="I57" s="2">
         <v>42953</v>
       </c>
     </row>
@@ -2645,7 +2650,7 @@
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="4">
         <v>42954</v>
       </c>
       <c r="C58" t="s">
@@ -2660,7 +2665,7 @@
       <c r="F58" t="s">
         <v>180</v>
       </c>
-      <c r="I58" s="6">
+      <c r="I58" s="2">
         <v>42954</v>
       </c>
     </row>
@@ -2669,7 +2674,7 @@
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="4">
         <v>42957</v>
       </c>
       <c r="C59" t="s">
@@ -2687,7 +2692,7 @@
       <c r="G59" t="s">
         <v>163</v>
       </c>
-      <c r="I59" s="6">
+      <c r="I59" s="2">
         <v>42957</v>
       </c>
     </row>
@@ -2696,7 +2701,7 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="4">
         <v>42960</v>
       </c>
       <c r="C60" t="s">
@@ -2711,7 +2716,7 @@
       <c r="F60" t="s">
         <v>181</v>
       </c>
-      <c r="I60" s="6">
+      <c r="I60" s="2">
         <v>42960</v>
       </c>
     </row>
@@ -2720,7 +2725,7 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61" s="4">
         <v>42962</v>
       </c>
       <c r="C61" t="s">
@@ -2738,7 +2743,7 @@
       <c r="G61" t="s">
         <v>166</v>
       </c>
-      <c r="I61" s="6">
+      <c r="I61" s="2">
         <v>42962</v>
       </c>
     </row>
@@ -2747,7 +2752,7 @@
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B62" s="4">
         <v>42963</v>
       </c>
       <c r="C62" t="s">
@@ -2762,7 +2767,7 @@
       <c r="F62" t="s">
         <v>239</v>
       </c>
-      <c r="I62" s="6">
+      <c r="I62" s="2">
         <v>42963</v>
       </c>
     </row>
@@ -2771,7 +2776,7 @@
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="4">
         <v>42972</v>
       </c>
       <c r="C63" t="s">
@@ -2789,7 +2794,7 @@
       <c r="G63" t="s">
         <v>184</v>
       </c>
-      <c r="I63" s="6">
+      <c r="I63" s="2">
         <v>42972</v>
       </c>
     </row>
@@ -2798,22 +2803,22 @@
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="B64" s="4">
+      <c r="B64" s="5">
         <v>42973</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E64" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F64" s="3" t="s">
+      <c r="E64" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="I64" s="7">
+      <c r="I64" s="3">
         <v>42973</v>
       </c>
     </row>
@@ -2822,19 +2827,19 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65" s="4">
         <v>42983</v>
       </c>
       <c r="C65" t="s">
         <v>73</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D65" s="1" t="s">
         <v>120</v>
       </c>
       <c r="E65" t="s">
         <v>2</v>
       </c>
-      <c r="I65" s="6">
+      <c r="I65" s="2">
         <v>42983</v>
       </c>
     </row>
@@ -2843,7 +2848,7 @@
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66" s="4">
         <v>42984</v>
       </c>
       <c r="C66" t="s">
@@ -2855,7 +2860,7 @@
       <c r="E66" t="s">
         <v>17</v>
       </c>
-      <c r="I66" s="6">
+      <c r="I66" s="2">
         <v>42984</v>
       </c>
     </row>
@@ -2864,7 +2869,7 @@
         <f t="shared" ref="A67:A106" si="1">ROW()-1</f>
         <v>66</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67" s="4">
         <v>42985</v>
       </c>
       <c r="C67" t="s">
@@ -2876,7 +2881,7 @@
       <c r="E67" t="s">
         <v>2</v>
       </c>
-      <c r="I67" s="6">
+      <c r="I67" s="2">
         <v>42985</v>
       </c>
     </row>
@@ -2885,7 +2890,7 @@
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68" s="4">
         <v>42988</v>
       </c>
       <c r="C68" t="s">
@@ -2900,7 +2905,7 @@
       <c r="F68" t="s">
         <v>260</v>
       </c>
-      <c r="I68" s="6">
+      <c r="I68" s="2">
         <v>42988</v>
       </c>
     </row>
@@ -2909,7 +2914,7 @@
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69" s="4">
         <v>42989</v>
       </c>
       <c r="C69" t="s">
@@ -2921,7 +2926,7 @@
       <c r="E69" t="s">
         <v>123</v>
       </c>
-      <c r="I69" s="6">
+      <c r="I69" s="2">
         <v>42989</v>
       </c>
     </row>
@@ -2930,7 +2935,7 @@
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70" s="4">
         <v>42993</v>
       </c>
       <c r="C70" t="s">
@@ -2945,7 +2950,7 @@
       <c r="F70" t="s">
         <v>270</v>
       </c>
-      <c r="I70" s="6">
+      <c r="I70" s="2">
         <v>42993</v>
       </c>
     </row>
@@ -2954,7 +2959,7 @@
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71" s="4">
         <v>42994</v>
       </c>
       <c r="C71" t="s">
@@ -2972,7 +2977,7 @@
       <c r="G71" t="s">
         <v>263</v>
       </c>
-      <c r="I71" s="6">
+      <c r="I71" s="2">
         <v>42994</v>
       </c>
     </row>
@@ -2981,7 +2986,7 @@
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="4">
         <v>42995</v>
       </c>
       <c r="C72" t="s">
@@ -2999,7 +3004,7 @@
       <c r="G72" t="s">
         <v>258</v>
       </c>
-      <c r="I72" s="6">
+      <c r="I72" s="2">
         <v>42995</v>
       </c>
     </row>
@@ -3008,7 +3013,7 @@
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B73" s="4">
         <v>42996</v>
       </c>
       <c r="C73" t="s">
@@ -3023,7 +3028,7 @@
       <c r="F73" t="s">
         <v>262</v>
       </c>
-      <c r="I73" s="6">
+      <c r="I73" s="2">
         <v>42996</v>
       </c>
     </row>
@@ -3032,7 +3037,7 @@
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74" s="4">
         <v>42999</v>
       </c>
       <c r="C74" t="s">
@@ -3047,7 +3052,7 @@
       <c r="F74" t="s">
         <v>256</v>
       </c>
-      <c r="I74" s="6">
+      <c r="I74" s="2">
         <v>42999</v>
       </c>
     </row>
@@ -3056,7 +3061,7 @@
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75" s="4">
         <v>43000</v>
       </c>
       <c r="C75" t="s">
@@ -3071,7 +3076,7 @@
       <c r="F75" t="s">
         <v>261</v>
       </c>
-      <c r="I75" s="6">
+      <c r="I75" s="2">
         <v>43000</v>
       </c>
     </row>
@@ -3080,7 +3085,7 @@
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76" s="4">
         <v>43001</v>
       </c>
       <c r="C76" t="s">
@@ -3098,7 +3103,7 @@
       <c r="G76" t="s">
         <v>255</v>
       </c>
-      <c r="I76" s="6">
+      <c r="I76" s="2">
         <v>43001</v>
       </c>
     </row>
@@ -3107,7 +3112,7 @@
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B77" s="4">
         <v>43002</v>
       </c>
       <c r="C77" t="s">
@@ -3122,7 +3127,7 @@
       <c r="F77" t="s">
         <v>252</v>
       </c>
-      <c r="I77" s="6">
+      <c r="I77" s="2">
         <v>43002</v>
       </c>
     </row>
@@ -3131,7 +3136,7 @@
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B78" s="4">
         <v>43006</v>
       </c>
       <c r="C78" t="s">
@@ -3149,7 +3154,7 @@
       <c r="G78" t="s">
         <v>269</v>
       </c>
-      <c r="I78" s="6">
+      <c r="I78" s="2">
         <v>43006</v>
       </c>
     </row>
@@ -3158,7 +3163,7 @@
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B79" s="4">
         <v>43009</v>
       </c>
       <c r="C79" t="s">
@@ -3173,7 +3178,7 @@
       <c r="F79" t="s">
         <v>251</v>
       </c>
-      <c r="I79" s="6">
+      <c r="I79" s="2">
         <v>43009</v>
       </c>
     </row>
@@ -3182,7 +3187,7 @@
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80" s="4">
         <v>43016</v>
       </c>
       <c r="C80" t="s">
@@ -3197,7 +3202,7 @@
       <c r="F80" t="s">
         <v>250</v>
       </c>
-      <c r="I80" s="6">
+      <c r="I80" s="2">
         <v>43016</v>
       </c>
     </row>
@@ -3206,7 +3211,7 @@
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B81" s="4">
         <v>43017</v>
       </c>
       <c r="C81" t="s">
@@ -3221,7 +3226,7 @@
       <c r="F81" t="s">
         <v>264</v>
       </c>
-      <c r="I81" s="6">
+      <c r="I81" s="2">
         <v>43017</v>
       </c>
     </row>
@@ -3230,7 +3235,7 @@
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B82" s="4">
         <v>43018</v>
       </c>
       <c r="C82" t="s">
@@ -3245,7 +3250,7 @@
       <c r="F82" t="s">
         <v>247</v>
       </c>
-      <c r="I82" s="6">
+      <c r="I82" s="2">
         <v>43018</v>
       </c>
     </row>
@@ -3254,7 +3259,7 @@
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B83" s="4">
         <v>43021</v>
       </c>
       <c r="C83" t="s">
@@ -3269,7 +3274,7 @@
       <c r="F83" t="s">
         <v>267</v>
       </c>
-      <c r="I83" s="6">
+      <c r="I83" s="2">
         <v>43021</v>
       </c>
     </row>
@@ -3278,7 +3283,7 @@
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B84" s="4">
         <v>43023</v>
       </c>
       <c r="C84" t="s">
@@ -3293,7 +3298,7 @@
       <c r="F84" t="s">
         <v>265</v>
       </c>
-      <c r="I84" s="6">
+      <c r="I84" s="2">
         <v>43023</v>
       </c>
     </row>
@@ -3302,7 +3307,7 @@
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-      <c r="B85" s="2">
+      <c r="B85" s="4">
         <v>43024</v>
       </c>
       <c r="C85" t="s">
@@ -3317,7 +3322,7 @@
       <c r="F85" t="s">
         <v>272</v>
       </c>
-      <c r="I85" s="6">
+      <c r="I85" s="2">
         <v>43024</v>
       </c>
     </row>
@@ -3326,7 +3331,7 @@
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B86" s="4">
         <v>43030</v>
       </c>
       <c r="C86" t="s">
@@ -3344,7 +3349,7 @@
       <c r="G86" t="s">
         <v>246</v>
       </c>
-      <c r="I86" s="6">
+      <c r="I86" s="2">
         <v>43030</v>
       </c>
     </row>
@@ -3353,7 +3358,7 @@
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B87" s="4">
         <v>43031</v>
       </c>
       <c r="C87" t="s">
@@ -3371,7 +3376,7 @@
       <c r="G87" t="s">
         <v>244</v>
       </c>
-      <c r="I87" s="6">
+      <c r="I87" s="2">
         <v>43031</v>
       </c>
     </row>
@@ -3380,7 +3385,7 @@
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B88" s="4">
         <v>43036</v>
       </c>
       <c r="C88" t="s">
@@ -3395,7 +3400,7 @@
       <c r="F88" t="s">
         <v>266</v>
       </c>
-      <c r="I88" s="6">
+      <c r="I88" s="2">
         <v>43036</v>
       </c>
     </row>
@@ -3404,7 +3409,7 @@
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B89" s="4">
         <v>43037</v>
       </c>
       <c r="C89" t="s">
@@ -3422,7 +3427,7 @@
       <c r="G89" t="s">
         <v>241</v>
       </c>
-      <c r="I89" s="6">
+      <c r="I89" s="2">
         <v>43037</v>
       </c>
     </row>
@@ -3431,7 +3436,7 @@
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B90" s="4">
         <v>43041</v>
       </c>
       <c r="C90" t="s">
@@ -3446,7 +3451,7 @@
       <c r="F90" t="s">
         <v>271</v>
       </c>
-      <c r="I90" s="6">
+      <c r="I90" s="2">
         <v>43041</v>
       </c>
     </row>
@@ -3458,19 +3463,19 @@
       <c r="B91" s="5">
         <v>43043</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="C91" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D91" s="3" t="s">
+      <c r="D91" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E91" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F91" s="3" t="s">
+      <c r="E91" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F91" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="I91" s="7">
+      <c r="I91" s="3">
         <v>43043</v>
       </c>
     </row>
@@ -3479,7 +3484,7 @@
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B92" s="4">
         <v>43049</v>
       </c>
       <c r="C92" t="s">
@@ -3494,7 +3499,7 @@
       <c r="F92" t="s">
         <v>185</v>
       </c>
-      <c r="I92" s="6">
+      <c r="I92" s="2">
         <v>43049</v>
       </c>
     </row>
@@ -3503,7 +3508,7 @@
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B93" s="4">
         <v>43057</v>
       </c>
       <c r="C93" t="s">
@@ -3518,7 +3523,7 @@
       <c r="F93" t="s">
         <v>167</v>
       </c>
-      <c r="I93" s="6">
+      <c r="I93" s="2">
         <v>43057</v>
       </c>
     </row>
@@ -3527,7 +3532,7 @@
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B94" s="4">
         <v>43059</v>
       </c>
       <c r="C94" t="s">
@@ -3545,7 +3550,7 @@
       <c r="G94" t="s">
         <v>186</v>
       </c>
-      <c r="I94" s="6">
+      <c r="I94" s="2">
         <v>43059</v>
       </c>
     </row>
@@ -3554,7 +3559,7 @@
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B95" s="4">
         <v>43060</v>
       </c>
       <c r="C95" t="s">
@@ -3569,7 +3574,7 @@
       <c r="F95" t="s">
         <v>192</v>
       </c>
-      <c r="I95" s="6">
+      <c r="I95" s="2">
         <v>43060</v>
       </c>
     </row>
@@ -3578,7 +3583,7 @@
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B96" s="4">
         <v>43062</v>
       </c>
       <c r="C96" t="s">
@@ -3593,7 +3598,7 @@
       <c r="F96" t="s">
         <v>168</v>
       </c>
-      <c r="I96" s="6">
+      <c r="I96" s="2">
         <v>43062</v>
       </c>
     </row>
@@ -3602,7 +3607,7 @@
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="B97" s="2">
+      <c r="B97" s="4">
         <v>43063</v>
       </c>
       <c r="C97" t="s">
@@ -3620,7 +3625,7 @@
       <c r="G97" t="s">
         <v>175</v>
       </c>
-      <c r="I97" s="6">
+      <c r="I97" s="2">
         <v>43063</v>
       </c>
     </row>
@@ -3629,7 +3634,7 @@
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
-      <c r="B98" s="2">
+      <c r="B98" s="4">
         <v>43064</v>
       </c>
       <c r="C98" t="s">
@@ -3644,7 +3649,7 @@
       <c r="F98" t="s">
         <v>214</v>
       </c>
-      <c r="I98" s="6">
+      <c r="I98" s="2">
         <v>43064</v>
       </c>
     </row>
@@ -3653,7 +3658,7 @@
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
-      <c r="B99" s="2">
+      <c r="B99" s="4">
         <v>43071</v>
       </c>
       <c r="C99" t="s">
@@ -3671,7 +3676,7 @@
       <c r="G99" t="s">
         <v>169</v>
       </c>
-      <c r="I99" s="6">
+      <c r="I99" s="2">
         <v>43071</v>
       </c>
     </row>
@@ -3680,7 +3685,7 @@
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
-      <c r="B100" s="2">
+      <c r="B100" s="4">
         <v>43072</v>
       </c>
       <c r="C100" t="s">
@@ -3698,7 +3703,7 @@
       <c r="G100" t="s">
         <v>224</v>
       </c>
-      <c r="I100" s="6">
+      <c r="I100" s="2">
         <v>43072</v>
       </c>
     </row>
@@ -3707,7 +3712,7 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="B101" s="2">
+      <c r="B101" s="4">
         <v>43075</v>
       </c>
       <c r="C101" t="s">
@@ -3719,7 +3724,7 @@
       <c r="E101" t="s">
         <v>2</v>
       </c>
-      <c r="I101" s="6">
+      <c r="I101" s="2">
         <v>43075</v>
       </c>
     </row>
@@ -3728,7 +3733,7 @@
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
-      <c r="B102" s="2">
+      <c r="B102" s="4">
         <v>43084</v>
       </c>
       <c r="C102" t="s">
@@ -3746,7 +3751,7 @@
       <c r="G102" t="s">
         <v>173</v>
       </c>
-      <c r="I102" s="6">
+      <c r="I102" s="2">
         <v>43084</v>
       </c>
     </row>
@@ -3755,7 +3760,7 @@
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
-      <c r="B103" s="2">
+      <c r="B103" s="4">
         <v>43085</v>
       </c>
       <c r="C103" t="s">
@@ -3773,7 +3778,7 @@
       <c r="G103" t="s">
         <v>171</v>
       </c>
-      <c r="I103" s="6">
+      <c r="I103" s="2">
         <v>43085</v>
       </c>
     </row>
@@ -3782,7 +3787,7 @@
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
-      <c r="B104" s="2">
+      <c r="B104" s="4">
         <v>43088</v>
       </c>
       <c r="C104" t="s">
@@ -3797,7 +3802,7 @@
       <c r="F104" t="s">
         <v>174</v>
       </c>
-      <c r="I104" s="6">
+      <c r="I104" s="2">
         <v>43088</v>
       </c>
     </row>
@@ -3806,7 +3811,7 @@
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
-      <c r="B105" s="2">
+      <c r="B105" s="4">
         <v>43093</v>
       </c>
       <c r="C105" t="s">
@@ -3821,7 +3826,7 @@
       <c r="F105" t="s">
         <v>281</v>
       </c>
-      <c r="I105" s="6">
+      <c r="I105" s="2">
         <v>43093</v>
       </c>
     </row>
@@ -3830,7 +3835,7 @@
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="B106" s="2">
+      <c r="B106" s="4">
         <v>43096</v>
       </c>
       <c r="C106" t="s">
@@ -3845,12 +3850,32 @@
       <c r="F106" t="s">
         <v>280</v>
       </c>
-      <c r="I106" s="6">
+      <c r="I106" s="2">
         <v>43096</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B107" s="2"/>
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" s="4">
+        <v>43099</v>
+      </c>
+      <c r="C107" t="s">
+        <v>40</v>
+      </c>
+      <c r="D107" t="s">
+        <v>292</v>
+      </c>
+      <c r="E107" t="s">
+        <v>42</v>
+      </c>
+      <c r="F107" t="s">
+        <v>291</v>
+      </c>
+      <c r="I107" s="2">
+        <v>43099</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated dates and sizes of flickr images
</commit_message>
<xml_diff>
--- a/posts/tapiocount_sheet.xlsx
+++ b/posts/tapiocount_sheet.xlsx
@@ -479,9 +479,6 @@
     <t>Sno-Crave</t>
   </si>
   <si>
-    <t>https://farm5.staticflickr.com/4691/38505051364_e9fd2b3e46_n.jpg</t>
-  </si>
-  <si>
     <t>https://farm5.staticflickr.com/4587/38505045714_d1b7224577_z.jpg</t>
   </si>
   <si>
@@ -551,201 +548,12 @@
     <t>https://farm5.staticflickr.com/4679/38336344555_06e1ed7806_z.jpg</t>
   </si>
   <si>
-    <t>https://farm5.staticflickr.com/4647/38505046574_a3be875bba_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4638/38336348275_f02bb482cd_b.jpg</t>
-  </si>
-  <si>
     <t>https://farm5.staticflickr.com/4727/38505047814_8f4889a723_z.jpg</t>
   </si>
   <si>
     <t>https://farm5.staticflickr.com/4688/38505045154_004d5a325d_z.jpg</t>
   </si>
   <si>
-    <t>https://farm5.staticflickr.com/4633/38336344965_29c34ee31b_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4596/38505047624_673b4b232b_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4638/38505047354_344440c92b_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4734/38336345195_8d2509d120_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4644/38505047194_92ffbe9c18_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4587/38336347635_939e3e4f37_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4690/24350573407_ed6dd089b3_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4738/38336347345_0697de2728_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4640/38505045004_103c5aff52_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4734/38336348975_39c6d5337b_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4596/38336345395_d39ee5fc83_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4595/38336349115_2b2f944568_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4645/38505048784_278b4122c4_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4725/38505046704_9aa28c7729_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4639/38336349215_14d8c01102_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4643/38505048954_41eddbf209_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4639/38336345455_aa57ef8194_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4646/38336349355_47aa904c25_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4733/38505049094_0792b162da_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4684/38505049284_1f3a99f822_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4591/38505049224_afc79abbb0_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4587/38336349605_4b61b6a6bc_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4735/38505049364_b61e6953e2_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4636/38505049454_722fe7536b_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4685/38336349835_b49635a716_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4600/38336345645_3799d0e21b_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4593/38505047704_0ee03b1a97_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4690/38505045524_405e2904a9_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4735/27436512779_e51f5abc3f_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4587/38505050084_6e4e582c52_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4739/38505050194_7eee884eb3_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4680/38505045644_81081e0fd8_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4735/24350573357_2a796d15af_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4733/38336345995_cfe7feff10_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4693/27436513349_424db03085_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4599/38505046474_cb18d85b59_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4690/38505050724_824cf0e69c_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4681/27436513619_40a1355729_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4639/38505050864_389229162b_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4591/27436513809_f06ce3b5d5_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4726/38505045754_03e1cc782b_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4633/38505051054_b397738c38_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4681/38336346175_9c2175e688_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4685/38336346895_acf55f5d53_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4730/38336346675_0942fecbe7_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4731/24350573327_1f78c01bb3_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4685/38505045874_fd8500fff2_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4739/38505051634_17c970eb1a_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4646/27436514369_92a0d57144_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4588/38336346285_9bd11eaa6e_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4683/38505045264_2e545b1789_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4637/24351971527_f0b4850bb4_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4686/38506601594_d7f4b2474e_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4735/24352057277_8c56bacd84_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4692/24352056737_7cd30c9295_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4589/24352055527_e1cfe74331_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4681/24352054427_13004ca608_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4634/39186409382_cf83fcdde1_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4643/39186409562_8ba382135d_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4646/39186409572_cedbae96e5_b.jpg</t>
-  </si>
-  <si>
-    <t>https://farm5.staticflickr.com/4634/24352183527_62be1eeb12_b.jpg</t>
-  </si>
-  <si>
     <t>https://farm5.staticflickr.com/4738/24352780527_d5cc4bc5c0_z.jpg</t>
   </si>
   <si>
@@ -903,6 +711,198 @@
   </si>
   <si>
     <t>The Yun Finest Green Tea</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4588/38336346285_9bd11eaa6e_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4646/27436514369_92a0d57144_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4739/38505051634_17c970eb1a_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4685/38505045874_fd8500fff2_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4633/38505051054_b397738c38_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4681/38336346175_9c2175e688_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4726/38505045754_03e1cc782b_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4591/27436513809_f06ce3b5d5_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4639/38505050864_389229162b_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4681/27436513619_40a1355729_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4690/38505050724_824cf0e69c_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4686/38506601594_d7f4b2474e_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4637/24351971527_f0b4850bb4_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4693/27436513349_424db03085_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4733/38336345995_cfe7feff10_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4680/38505045644_81081e0fd8_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4681/24352054427_13004ca608_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4739/38505050194_7eee884eb3_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4587/38505050084_6e4e582c52_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4735/27436512779_e51f5abc3f_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4692/24352056737_7cd30c9295_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4735/24352057277_8c56bacd84_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4589/24352055527_e1cfe74331_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4690/38505045524_405e2904a9_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4646/39186409572_cedbae96e5_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4643/39186409562_8ba382135d_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4634/39186409382_cf83fcdde1_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4600/38336345645_3799d0e21b_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4685/38336349835_b49635a716_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4636/38505049454_722fe7536b_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4735/38505049364_b61e6953e2_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4591/38505049224_afc79abbb0_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4587/38336349605_4b61b6a6bc_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4684/38505049284_1f3a99f822_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4733/38505049094_0792b162da_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4646/38336349355_47aa904c25_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4639/38336345455_aa57ef8194_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4643/38505048954_41eddbf209_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4683/38505045264_2e545b1789_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4639/38336349215_14d8c01102_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4595/38336349115_2b2f944568_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4645/38505048784_278b4122c4_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4596/38336345395_d39ee5fc83_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4734/38336348975_39c6d5337b_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4734/38336345195_8d2509d120_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4593/38505047704_0ee03b1a97_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4638/38336348275_f02bb482cd_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4633/38336344965_29c34ee31b_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4596/38505047624_673b4b232b_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4638/38505047354_344440c92b_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4634/24352183527_62be1eeb12_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4644/38505047194_92ffbe9c18_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4587/38336347635_939e3e4f37_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4690/24350573407_ed6dd089b3_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4640/38505045004_103c5aff52_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4738/38336347345_0697de2728_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4725/38505046704_9aa28c7729_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4735/24350573357_2a796d15af_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4647/38505046574_a3be875bba_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4599/38505046474_cb18d85b59_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4685/38336346895_acf55f5d53_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4730/38336346675_0942fecbe7_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4731/24350573327_1f78c01bb3_z.jpg</t>
+  </si>
+  <si>
+    <t>https://farm5.staticflickr.com/4691/38505051364_e9fd2b3e46_z.jpg</t>
   </si>
 </sst>
 </file>
@@ -910,8 +910,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="mmmm\ d"/>
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="mmmm\ d"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -951,10 +951,10 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1234,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1244,38 +1244,38 @@
     <col min="3" max="3" width="20.1640625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>282</v>
+        <v>218</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>283</v>
+        <v>219</v>
       </c>
       <c r="C1" t="s">
-        <v>284</v>
+        <v>220</v>
       </c>
       <c r="D1" t="s">
-        <v>285</v>
+        <v>221</v>
       </c>
       <c r="E1" t="s">
-        <v>286</v>
+        <v>222</v>
       </c>
       <c r="F1" t="s">
-        <v>287</v>
+        <v>223</v>
       </c>
       <c r="G1" t="s">
-        <v>288</v>
+        <v>224</v>
       </c>
       <c r="H1" t="s">
-        <v>289</v>
+        <v>225</v>
       </c>
       <c r="I1" t="s">
-        <v>290</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1371,7 +1371,7 @@
         <v>42769</v>
       </c>
       <c r="C6" t="s">
-        <v>275</v>
+        <v>211</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -1380,10 +1380,10 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G6" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="I6" s="2">
         <v>42769</v>
@@ -1470,7 +1470,7 @@
         <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="I10" s="2">
         <v>42779</v>
@@ -1494,7 +1494,7 @@
         <v>17</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1520,7 +1520,7 @@
         <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>151</v>
+        <v>292</v>
       </c>
       <c r="I12" s="2">
         <v>42791</v>
@@ -1544,10 +1544,10 @@
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="G13" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="I13" s="2">
         <v>42798</v>
@@ -1571,7 +1571,7 @@
         <v>26</v>
       </c>
       <c r="F14" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="I14" s="2">
         <v>42804</v>
@@ -1595,7 +1595,7 @@
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>218</v>
+        <v>236</v>
       </c>
       <c r="I15" s="2">
         <v>42805</v>
@@ -1619,7 +1619,7 @@
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="I16" s="2">
         <v>42806</v>
@@ -1643,7 +1643,7 @@
         <v>31</v>
       </c>
       <c r="F17" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="I17" s="2">
         <v>42812</v>
@@ -1667,10 +1667,10 @@
         <v>34</v>
       </c>
       <c r="F18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G18" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="I18" s="2">
         <v>42813</v>
@@ -1694,10 +1694,10 @@
         <v>36</v>
       </c>
       <c r="F19" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="G19" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="I19" s="2">
         <v>42817</v>
@@ -1721,7 +1721,7 @@
         <v>2</v>
       </c>
       <c r="F20" t="s">
-        <v>213</v>
+        <v>242</v>
       </c>
       <c r="I20" s="2">
         <v>42829</v>
@@ -1766,10 +1766,10 @@
         <v>42</v>
       </c>
       <c r="F22" t="s">
-        <v>212</v>
+        <v>243</v>
       </c>
       <c r="G22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I22" s="2">
         <v>42834</v>
@@ -1793,10 +1793,10 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
+        <v>244</v>
+      </c>
+      <c r="G23" t="s">
         <v>210</v>
-      </c>
-      <c r="G23" t="s">
-        <v>274</v>
       </c>
       <c r="I23" s="2">
         <v>42835</v>
@@ -1820,7 +1820,7 @@
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="I24" s="2">
         <v>42836</v>
@@ -1844,7 +1844,7 @@
         <v>128</v>
       </c>
       <c r="F25" t="s">
-        <v>209</v>
+        <v>246</v>
       </c>
       <c r="I25" s="2">
         <v>42846</v>
@@ -1868,7 +1868,7 @@
         <v>50</v>
       </c>
       <c r="F26" t="s">
-        <v>208</v>
+        <v>247</v>
       </c>
       <c r="I26" s="2">
         <v>42848</v>
@@ -1892,10 +1892,10 @@
         <v>53</v>
       </c>
       <c r="F27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G27" t="s">
-        <v>207</v>
+        <v>248</v>
       </c>
       <c r="I27" s="2">
         <v>42854</v>
@@ -1919,7 +1919,7 @@
         <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
       <c r="I28" s="2">
         <v>42855</v>
@@ -1943,10 +1943,10 @@
         <v>26</v>
       </c>
       <c r="F29" t="s">
-        <v>232</v>
+        <v>250</v>
       </c>
       <c r="G29" t="s">
-        <v>234</v>
+        <v>251</v>
       </c>
       <c r="I29" s="2">
         <v>42870</v>
@@ -1970,7 +1970,7 @@
         <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>206</v>
+        <v>252</v>
       </c>
       <c r="I30" s="2">
         <v>42877</v>
@@ -1994,7 +1994,7 @@
         <v>59</v>
       </c>
       <c r="F31" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="I31" s="2">
         <v>42880</v>
@@ -2018,7 +2018,7 @@
         <v>62</v>
       </c>
       <c r="F32" t="s">
-        <v>237</v>
+        <v>254</v>
       </c>
       <c r="I32" s="2">
         <v>42881</v>
@@ -2042,7 +2042,7 @@
         <v>64</v>
       </c>
       <c r="F33" t="s">
-        <v>236</v>
+        <v>255</v>
       </c>
       <c r="I33" s="2">
         <v>42890</v>
@@ -2066,7 +2066,7 @@
         <v>17</v>
       </c>
       <c r="F34" t="s">
-        <v>204</v>
+        <v>256</v>
       </c>
       <c r="I34" s="2">
         <v>42891</v>
@@ -2090,7 +2090,7 @@
         <v>2</v>
       </c>
       <c r="F35" t="s">
-        <v>203</v>
+        <v>257</v>
       </c>
       <c r="I35" s="2">
         <v>42891</v>
@@ -2114,7 +2114,7 @@
         <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>202</v>
+        <v>258</v>
       </c>
       <c r="I36" s="2">
         <v>42897</v>
@@ -2138,7 +2138,7 @@
         <v>2</v>
       </c>
       <c r="F37" t="s">
-        <v>201</v>
+        <v>259</v>
       </c>
       <c r="I37" s="2">
         <v>42899</v>
@@ -2162,10 +2162,10 @@
         <v>2</v>
       </c>
       <c r="F38" t="s">
-        <v>199</v>
+        <v>260</v>
       </c>
       <c r="G38" t="s">
-        <v>200</v>
+        <v>261</v>
       </c>
       <c r="I38" s="2">
         <v>42901</v>
@@ -2189,7 +2189,7 @@
         <v>17</v>
       </c>
       <c r="F39" t="s">
-        <v>198</v>
+        <v>262</v>
       </c>
       <c r="I39" s="2">
         <v>42902</v>
@@ -2213,7 +2213,7 @@
         <v>17</v>
       </c>
       <c r="F40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I40" s="2">
         <v>42904</v>
@@ -2237,7 +2237,7 @@
         <v>2</v>
       </c>
       <c r="F41" t="s">
-        <v>197</v>
+        <v>263</v>
       </c>
       <c r="I41" s="2">
         <v>42914</v>
@@ -2261,10 +2261,10 @@
         <v>17</v>
       </c>
       <c r="F42" t="s">
-        <v>196</v>
+        <v>264</v>
       </c>
       <c r="G42" t="s">
-        <v>195</v>
+        <v>265</v>
       </c>
       <c r="I42" s="2">
         <v>42918</v>
@@ -2288,7 +2288,7 @@
         <v>2</v>
       </c>
       <c r="F43" t="s">
-        <v>194</v>
+        <v>266</v>
       </c>
       <c r="I43" s="2">
         <v>42919</v>
@@ -2312,10 +2312,10 @@
         <v>34</v>
       </c>
       <c r="F44" t="s">
-        <v>229</v>
+        <v>267</v>
       </c>
       <c r="G44" t="s">
-        <v>193</v>
+        <v>268</v>
       </c>
       <c r="I44" s="2">
         <v>42920</v>
@@ -2360,10 +2360,10 @@
         <v>17</v>
       </c>
       <c r="F46" t="s">
-        <v>190</v>
+        <v>269</v>
       </c>
       <c r="G46" t="s">
-        <v>191</v>
+        <v>270</v>
       </c>
       <c r="I46" s="2">
         <v>42926</v>
@@ -2387,7 +2387,7 @@
         <v>2</v>
       </c>
       <c r="F47" t="s">
-        <v>189</v>
+        <v>271</v>
       </c>
       <c r="I47" s="2">
         <v>42927</v>
@@ -2411,10 +2411,10 @@
         <v>2</v>
       </c>
       <c r="F48" t="s">
-        <v>188</v>
+        <v>272</v>
       </c>
       <c r="G48" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I48" s="2">
         <v>42929</v>
@@ -2438,10 +2438,10 @@
         <v>2</v>
       </c>
       <c r="F49" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I49" s="2">
         <v>42930</v>
@@ -2465,10 +2465,10 @@
         <v>80</v>
       </c>
       <c r="F50" t="s">
-        <v>273</v>
+        <v>209</v>
       </c>
       <c r="G50" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I50" s="2">
         <v>42932</v>
@@ -2492,7 +2492,7 @@
         <v>2</v>
       </c>
       <c r="F51" t="s">
-        <v>182</v>
+        <v>273</v>
       </c>
       <c r="I51" s="2">
         <v>42934</v>
@@ -2516,7 +2516,7 @@
         <v>2</v>
       </c>
       <c r="F52" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I52" s="2">
         <v>42936</v>
@@ -2540,10 +2540,10 @@
         <v>2</v>
       </c>
       <c r="F53" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G53" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I53" s="2">
         <v>42940</v>
@@ -2567,7 +2567,7 @@
         <v>83</v>
       </c>
       <c r="F54" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I54" s="2">
         <v>42945</v>
@@ -2591,7 +2591,7 @@
         <v>85</v>
       </c>
       <c r="F55" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="I55" s="2">
         <v>42951</v>
@@ -2615,7 +2615,7 @@
         <v>87</v>
       </c>
       <c r="F56" t="s">
-        <v>176</v>
+        <v>275</v>
       </c>
       <c r="I56" s="2">
         <v>42951</v>
@@ -2639,7 +2639,7 @@
         <v>90</v>
       </c>
       <c r="F57" t="s">
-        <v>179</v>
+        <v>276</v>
       </c>
       <c r="I57" s="2">
         <v>42953</v>
@@ -2663,7 +2663,7 @@
         <v>93</v>
       </c>
       <c r="F58" t="s">
-        <v>180</v>
+        <v>277</v>
       </c>
       <c r="I58" s="2">
         <v>42954</v>
@@ -2687,10 +2687,10 @@
         <v>2</v>
       </c>
       <c r="F59" t="s">
+        <v>161</v>
+      </c>
+      <c r="G59" t="s">
         <v>162</v>
-      </c>
-      <c r="G59" t="s">
-        <v>163</v>
       </c>
       <c r="I59" s="2">
         <v>42957</v>
@@ -2714,7 +2714,7 @@
         <v>2</v>
       </c>
       <c r="F60" t="s">
-        <v>181</v>
+        <v>278</v>
       </c>
       <c r="I60" s="2">
         <v>42960</v>
@@ -2738,10 +2738,10 @@
         <v>95</v>
       </c>
       <c r="F61" t="s">
+        <v>164</v>
+      </c>
+      <c r="G61" t="s">
         <v>165</v>
-      </c>
-      <c r="G61" t="s">
-        <v>166</v>
       </c>
       <c r="I61" s="2">
         <v>42962</v>
@@ -2765,7 +2765,7 @@
         <v>2</v>
       </c>
       <c r="F62" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="I62" s="2">
         <v>42963</v>
@@ -2789,10 +2789,10 @@
         <v>2</v>
       </c>
       <c r="F63" t="s">
-        <v>183</v>
+        <v>280</v>
       </c>
       <c r="G63" t="s">
-        <v>184</v>
+        <v>281</v>
       </c>
       <c r="I63" s="2">
         <v>42972</v>
@@ -2816,7 +2816,7 @@
         <v>2</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I64" s="3">
         <v>42973</v>
@@ -2903,7 +2903,7 @@
         <v>124</v>
       </c>
       <c r="F68" t="s">
-        <v>260</v>
+        <v>196</v>
       </c>
       <c r="I68" s="2">
         <v>42988</v>
@@ -2948,7 +2948,7 @@
         <v>2</v>
       </c>
       <c r="F70" t="s">
-        <v>270</v>
+        <v>206</v>
       </c>
       <c r="I70" s="2">
         <v>42993</v>
@@ -2972,10 +2972,10 @@
         <v>126</v>
       </c>
       <c r="F71" t="s">
-        <v>259</v>
+        <v>195</v>
       </c>
       <c r="G71" t="s">
-        <v>263</v>
+        <v>199</v>
       </c>
       <c r="I71" s="2">
         <v>42994</v>
@@ -2999,10 +2999,10 @@
         <v>2</v>
       </c>
       <c r="F72" t="s">
-        <v>257</v>
+        <v>193</v>
       </c>
       <c r="G72" t="s">
-        <v>258</v>
+        <v>194</v>
       </c>
       <c r="I72" s="2">
         <v>42995</v>
@@ -3026,7 +3026,7 @@
         <v>128</v>
       </c>
       <c r="F73" t="s">
-        <v>262</v>
+        <v>198</v>
       </c>
       <c r="I73" s="2">
         <v>42996</v>
@@ -3050,7 +3050,7 @@
         <v>2</v>
       </c>
       <c r="F74" t="s">
-        <v>256</v>
+        <v>192</v>
       </c>
       <c r="I74" s="2">
         <v>42999</v>
@@ -3074,7 +3074,7 @@
         <v>2</v>
       </c>
       <c r="F75" t="s">
-        <v>261</v>
+        <v>197</v>
       </c>
       <c r="I75" s="2">
         <v>43000</v>
@@ -3098,10 +3098,10 @@
         <v>2</v>
       </c>
       <c r="F76" t="s">
-        <v>254</v>
+        <v>190</v>
       </c>
       <c r="G76" t="s">
-        <v>255</v>
+        <v>191</v>
       </c>
       <c r="I76" s="2">
         <v>43001</v>
@@ -3119,13 +3119,13 @@
         <v>8</v>
       </c>
       <c r="D77" t="s">
-        <v>253</v>
+        <v>189</v>
       </c>
       <c r="E77" t="s">
         <v>34</v>
       </c>
       <c r="F77" t="s">
-        <v>252</v>
+        <v>188</v>
       </c>
       <c r="I77" s="2">
         <v>43002</v>
@@ -3149,10 +3149,10 @@
         <v>132</v>
       </c>
       <c r="F78" t="s">
-        <v>268</v>
+        <v>204</v>
       </c>
       <c r="G78" t="s">
-        <v>269</v>
+        <v>205</v>
       </c>
       <c r="I78" s="2">
         <v>43006</v>
@@ -3176,7 +3176,7 @@
         <v>133</v>
       </c>
       <c r="F79" t="s">
-        <v>251</v>
+        <v>187</v>
       </c>
       <c r="I79" s="2">
         <v>43009</v>
@@ -3191,16 +3191,16 @@
         <v>43016</v>
       </c>
       <c r="C80" t="s">
-        <v>248</v>
+        <v>184</v>
       </c>
       <c r="D80" t="s">
         <v>121</v>
       </c>
       <c r="E80" t="s">
-        <v>249</v>
+        <v>185</v>
       </c>
       <c r="F80" t="s">
-        <v>250</v>
+        <v>186</v>
       </c>
       <c r="I80" s="2">
         <v>43016</v>
@@ -3224,7 +3224,7 @@
         <v>138</v>
       </c>
       <c r="F81" t="s">
-        <v>264</v>
+        <v>200</v>
       </c>
       <c r="I81" s="2">
         <v>43017</v>
@@ -3248,7 +3248,7 @@
         <v>138</v>
       </c>
       <c r="F82" t="s">
-        <v>247</v>
+        <v>183</v>
       </c>
       <c r="I82" s="2">
         <v>43018</v>
@@ -3272,7 +3272,7 @@
         <v>17</v>
       </c>
       <c r="F83" t="s">
-        <v>267</v>
+        <v>203</v>
       </c>
       <c r="I83" s="2">
         <v>43021</v>
@@ -3296,7 +3296,7 @@
         <v>107</v>
       </c>
       <c r="F84" t="s">
-        <v>265</v>
+        <v>201</v>
       </c>
       <c r="I84" s="2">
         <v>43023</v>
@@ -3320,7 +3320,7 @@
         <v>123</v>
       </c>
       <c r="F85" t="s">
-        <v>272</v>
+        <v>208</v>
       </c>
       <c r="I85" s="2">
         <v>43024</v>
@@ -3344,10 +3344,10 @@
         <v>2</v>
       </c>
       <c r="F86" t="s">
-        <v>245</v>
+        <v>181</v>
       </c>
       <c r="G86" t="s">
-        <v>246</v>
+        <v>182</v>
       </c>
       <c r="I86" s="2">
         <v>43030</v>
@@ -3371,10 +3371,10 @@
         <v>2</v>
       </c>
       <c r="F87" t="s">
-        <v>243</v>
+        <v>179</v>
       </c>
       <c r="G87" t="s">
-        <v>244</v>
+        <v>180</v>
       </c>
       <c r="I87" s="2">
         <v>43031</v>
@@ -3398,7 +3398,7 @@
         <v>50</v>
       </c>
       <c r="F88" t="s">
-        <v>266</v>
+        <v>202</v>
       </c>
       <c r="I88" s="2">
         <v>43036</v>
@@ -3422,10 +3422,10 @@
         <v>34</v>
       </c>
       <c r="F89" t="s">
-        <v>242</v>
+        <v>178</v>
       </c>
       <c r="G89" t="s">
-        <v>241</v>
+        <v>177</v>
       </c>
       <c r="I89" s="2">
         <v>43037</v>
@@ -3449,7 +3449,7 @@
         <v>2</v>
       </c>
       <c r="F90" t="s">
-        <v>271</v>
+        <v>207</v>
       </c>
       <c r="I90" s="2">
         <v>43041</v>
@@ -3473,7 +3473,7 @@
         <v>2</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>240</v>
+        <v>176</v>
       </c>
       <c r="I91" s="3">
         <v>43043</v>
@@ -3488,7 +3488,7 @@
         <v>43049</v>
       </c>
       <c r="C92" t="s">
-        <v>276</v>
+        <v>212</v>
       </c>
       <c r="D92" t="s">
         <v>146</v>
@@ -3497,7 +3497,7 @@
         <v>2</v>
       </c>
       <c r="F92" t="s">
-        <v>185</v>
+        <v>282</v>
       </c>
       <c r="I92" s="2">
         <v>43049</v>
@@ -3521,7 +3521,7 @@
         <v>2</v>
       </c>
       <c r="F93" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I93" s="2">
         <v>43057</v>
@@ -3545,10 +3545,10 @@
         <v>2</v>
       </c>
       <c r="F94" t="s">
-        <v>187</v>
+        <v>283</v>
       </c>
       <c r="G94" t="s">
-        <v>186</v>
+        <v>284</v>
       </c>
       <c r="I94" s="2">
         <v>43059</v>
@@ -3572,7 +3572,7 @@
         <v>2</v>
       </c>
       <c r="F95" t="s">
-        <v>192</v>
+        <v>285</v>
       </c>
       <c r="I95" s="2">
         <v>43060</v>
@@ -3596,7 +3596,7 @@
         <v>2</v>
       </c>
       <c r="F96" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I96" s="2">
         <v>43062</v>
@@ -3620,10 +3620,10 @@
         <v>19</v>
       </c>
       <c r="F97" t="s">
-        <v>211</v>
+        <v>286</v>
       </c>
       <c r="G97" t="s">
-        <v>175</v>
+        <v>287</v>
       </c>
       <c r="I97" s="2">
         <v>43063</v>
@@ -3647,7 +3647,7 @@
         <v>149</v>
       </c>
       <c r="F98" t="s">
-        <v>214</v>
+        <v>288</v>
       </c>
       <c r="I98" s="2">
         <v>43064</v>
@@ -3671,10 +3671,10 @@
         <v>107</v>
       </c>
       <c r="F99" t="s">
-        <v>222</v>
+        <v>289</v>
       </c>
       <c r="G99" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I99" s="2">
         <v>43071</v>
@@ -3698,10 +3698,10 @@
         <v>105</v>
       </c>
       <c r="F100" t="s">
-        <v>223</v>
+        <v>290</v>
       </c>
       <c r="G100" t="s">
-        <v>224</v>
+        <v>291</v>
       </c>
       <c r="I100" s="2">
         <v>43072</v>
@@ -3746,10 +3746,10 @@
         <v>2</v>
       </c>
       <c r="F102" t="s">
+        <v>171</v>
+      </c>
+      <c r="G102" t="s">
         <v>172</v>
-      </c>
-      <c r="G102" t="s">
-        <v>173</v>
       </c>
       <c r="I102" s="2">
         <v>43084</v>
@@ -3773,10 +3773,10 @@
         <v>101</v>
       </c>
       <c r="F103" t="s">
+        <v>169</v>
+      </c>
+      <c r="G103" t="s">
         <v>170</v>
-      </c>
-      <c r="G103" t="s">
-        <v>171</v>
       </c>
       <c r="I103" s="2">
         <v>43085</v>
@@ -3800,7 +3800,7 @@
         <v>17</v>
       </c>
       <c r="F104" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I104" s="2">
         <v>43088</v>
@@ -3818,13 +3818,13 @@
         <v>68</v>
       </c>
       <c r="D105" t="s">
-        <v>277</v>
+        <v>213</v>
       </c>
       <c r="E105" t="s">
         <v>2</v>
       </c>
       <c r="F105" t="s">
-        <v>281</v>
+        <v>217</v>
       </c>
       <c r="I105" s="2">
         <v>43093</v>
@@ -3842,13 +3842,13 @@
         <v>30</v>
       </c>
       <c r="D106" t="s">
-        <v>278</v>
+        <v>214</v>
       </c>
       <c r="E106" t="s">
-        <v>279</v>
+        <v>215</v>
       </c>
       <c r="F106" t="s">
-        <v>280</v>
+        <v>216</v>
       </c>
       <c r="I106" s="2">
         <v>43096</v>
@@ -3865,13 +3865,13 @@
         <v>40</v>
       </c>
       <c r="D107" t="s">
-        <v>292</v>
+        <v>228</v>
       </c>
       <c r="E107" t="s">
         <v>42</v>
       </c>
       <c r="F107" t="s">
-        <v>291</v>
+        <v>227</v>
       </c>
       <c r="I107" s="2">
         <v>43099</v>

</xml_diff>